<commit_message>
Adrian Peterson twitter data from trade phases
</commit_message>
<xml_diff>
--- a/Player Historical Trade Tweets/Data Tracker/Fixed Data.xlsx
+++ b/Player Historical Trade Tweets/Data Tracker/Fixed Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\rprezzano\Work Folders\Desktop\fixed_duplicates\GetOldTweets-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\rprezzano\Work Folders\Desktop\project-seadogs\Player Historical Trade Tweets\Data Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -135,7 +135,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,13 +144,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3300"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,9 +198,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +489,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -517,136 +523,136 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="10">
         <v>38837</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="10">
         <f>B2-7</f>
         <v>38830</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="10">
         <f>B2+7</f>
         <v>38844</v>
       </c>
-      <c r="F2" s="7" t="str">
+      <c r="F2" s="9" t="str">
         <f>CONCATENATE("python Exporter.py --querysearch ",CHAR(34),A2,CHAR(34)," --since ",TEXT(D2,"yyyy-mm-dd")," --until ",TEXT(E2,"yyyy-mm-dd")," --maxtweets 1000000")</f>
         <v>python Exporter.py --querysearch "Brandon Marshall" --since 2006-04-23 --until 2006-05-07 --maxtweets 1000000</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>40282</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>40275</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="8">
         <v>40289</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>40981</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>40974</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>40988</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>42073</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>42066</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="8">
         <v>42080</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="8">
         <v>42802</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>42795</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="8">
         <v>42809</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <v>39200</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>39193</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>39207</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3">

</xml_diff>